<commit_message>
Added and Updated WB tests for getSpaceRemaining and sortByLimitingFactor
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_getSpaceRemaining.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_getSpaceRemaining.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intae\Documents\1_Seneca\Sem2\sft221\Group Project\SUM23-SFT221-NAA-4\Documents\Testing\TestsDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDD531E-A2A6-46BF-B21E-45C1DACBA4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A425023F-A1CA-4EC7-BEE6-153A5934BC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="825" windowWidth="14475" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13785" yWindow="2175" windowWidth="14475" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>SFT 221</t>
   </si>
@@ -170,22 +170,41 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>Pointer to Truck is a null pointer</t>
-  </si>
-  <si>
-    <t>Function should handle null pointers without causing runtime issues</t>
-  </si>
-  <si>
     <t>0.0</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>Exception Code: C0000005</t>
+    <t>truck.CurrentWeight = 0
+truck.CurrentVolume = 0</t>
+  </si>
+  <si>
+    <t>truck.CurrentWeight = 500
+truck.CurrentVolume = 18</t>
+  </si>
+  <si>
+    <t>Check function returns the correct result if truck is exactly half full</t>
+  </si>
+  <si>
+    <t>Check function returns the correct result if truck is empty</t>
+  </si>
+  <si>
+    <t>truck.CurrentWeight = 1
+truck.CurrentVolume = 0.25</t>
+  </si>
+  <si>
+    <t>Check function returns the correct result if truck has the tiniest possible package</t>
+  </si>
+  <si>
+    <t>truck.CurrentWeight = 999
+truck.CurrentVolume = 35.75</t>
+  </si>
+  <si>
+    <t>Check if function returns the correct result if truck has the maximum possible load with a little bit of space remaining.</t>
+  </si>
+  <si>
+    <t>(36 - 0.25) / 36 = 0.9930555555555;</t>
   </si>
 </sst>
 </file>
@@ -223,13 +242,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,12 +284,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -425,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -457,6 +469,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -505,11 +520,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,116 +821,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="23">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -920,17 +938,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -953,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,15 +985,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1016,8 +1034,8 @@
       <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>42</v>
+      <c r="G3" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1036,8 +1054,8 @@
       <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="29" t="s">
-        <v>42</v>
+      <c r="G4" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1051,13 +1069,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="29" t="s">
-        <v>42</v>
+      <c r="G5" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1071,13 +1089,13 @@
         <v>26</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>42</v>
+      <c r="G6" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1096,8 +1114,8 @@
       <c r="E7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="29" t="s">
-        <v>42</v>
+      <c r="G7" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1116,8 +1134,8 @@
       <c r="E8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="29" t="s">
-        <v>42</v>
+      <c r="G8" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1136,8 +1154,8 @@
       <c r="E9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="29" t="s">
-        <v>42</v>
+      <c r="G9" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1156,8 +1174,8 @@
       <c r="E10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>42</v>
+      <c r="G10" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1279,28 +1297,28 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="65.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="56.140625" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1332,30 +1350,78 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>39</v>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="3"/>
+      <c r="G4" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
@@ -1483,12 +1549,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1663,15 +1726,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1696,18 +1771,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed test case names to reflect test code for getSpaceRemaining and sortByLimitingFactor
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_getSpaceRemaining.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_getSpaceRemaining.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intae\Documents\1_Seneca\Sem2\sft221\Group Project\SUM23-SFT221-NAA-4\Documents\Testing\TestsDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A425023F-A1CA-4EC7-BEE6-153A5934BC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AD3526-6A3B-44B0-AF3C-DDD6EA760FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="2175" windowWidth="14475" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="870" windowWidth="14475" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>SFT 221</t>
   </si>
@@ -205,6 +205,52 @@
   </si>
   <si>
     <t>(36 - 0.25) / 36 = 0.9930555555555;</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining1</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining2</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining3</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining4</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining5</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining6</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining7</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining8</t>
+  </si>
+  <si>
+    <t>BB_TestGetSpaceRemaining9</t>
+  </si>
+  <si>
+    <t>truck.CurrentWeight =  1000
+truck.CurrentVolume = 24</t>
+  </si>
+  <si>
+    <t>Check function returns the correct result if CurrentVolume is not full but CurrentWeight is</t>
+  </si>
+  <si>
+    <t>WB_TestGetSpaceRemaining1</t>
+  </si>
+  <si>
+    <t>WB_TestGetSpaceRemaining2</t>
+  </si>
+  <si>
+    <t>WB_TestGetSpaceRemaining3</t>
+  </si>
+  <si>
+    <t>WB_TestGetSpaceRemaining4</t>
   </si>
 </sst>
 </file>
@@ -437,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -472,6 +518,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,15 +570,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -821,116 +864,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="25">
         <v>4</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
     </row>
     <row r="9" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -938,17 +981,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -971,13 +1014,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="56.140625" customWidth="1"/>
@@ -985,15 +1029,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1019,8 +1063,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
+      <c r="A3" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1039,8 +1083,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
+      <c r="A4" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1059,8 +1103,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
+      <c r="A5" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1079,8 +1123,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>4</v>
+      <c r="A6" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1099,8 +1143,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>5</v>
+      <c r="A7" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1119,8 +1163,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>6</v>
+      <c r="A8" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1139,8 +1183,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>7</v>
+      <c r="A9" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1159,8 +1203,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>8</v>
+      <c r="A10" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1178,8 +1222,25 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="3"/>
+    <row r="11" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
@@ -1296,13 +1357,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="56.140625" customWidth="1"/>
@@ -1310,15 +1372,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1344,8 +1406,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1</v>
+      <c r="A3" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1359,13 +1421,13 @@
       <c r="E3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
+      <c r="A4" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1379,13 +1441,13 @@
       <c r="E4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="30" t="s">
+      <c r="G4" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>3</v>
+      <c r="A5" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -1393,19 +1455,19 @@
       <c r="C5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="15" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="14" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
-        <v>4</v>
+      <c r="A6" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1419,7 +1481,7 @@
       <c r="E6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="14" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1549,9 +1611,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1726,27 +1791,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1771,9 +1824,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated test names for getSpaceRemaining and sortByLimitingFactor
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_getSpaceRemaining.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_getSpaceRemaining.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intae\Documents\1_Seneca\Sem2\sft221\Group Project\SUM23-SFT221-NAA-4\Documents\Testing\TestsDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AD3526-6A3B-44B0-AF3C-DDD6EA760FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D28560B-8B42-4260-8505-36C16164ED83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="870" windowWidth="14475" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="690" windowWidth="14475" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1357,7 +1357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1611,12 +1611,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1791,15 +1788,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1824,18 +1833,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>